<commit_message>
end to end testing, also file generator added
</commit_message>
<xml_diff>
--- a/testData/TestData.xlsx
+++ b/testData/TestData.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sinut001\Documents\Automation Projects\Automation Projects\Web\AdactinHotelCucumberBDDFramework\AdactinHotelCucumberBDDFramework\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB08200E-7AE4-4DD3-BD5E-45464907D462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6A307B-C9EA-41B8-B8BF-C1CB8A8BA20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
+    <sheet name="SearchHotel" sheetId="2" r:id="rId2"/>
+    <sheet name="BillingInformation" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Username</t>
   </si>
@@ -37,6 +39,102 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Hotels</t>
+  </si>
+  <si>
+    <t>RoomType</t>
+  </si>
+  <si>
+    <t>NumberOfRooms</t>
+  </si>
+  <si>
+    <t>CheckInDate</t>
+  </si>
+  <si>
+    <t>CheckOutDate</t>
+  </si>
+  <si>
+    <t>ChildrenPerRoom</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Hotel Cornice</t>
+  </si>
+  <si>
+    <t>Super Deluxe</t>
+  </si>
+  <si>
+    <t>28/01/2024</t>
+  </si>
+  <si>
+    <t>08/02/2024</t>
+  </si>
+  <si>
+    <t>2 - Two</t>
+  </si>
+  <si>
+    <t>1 - One</t>
+  </si>
+  <si>
+    <t>AdultsPerRoom</t>
+  </si>
+  <si>
+    <t>7 - Seven</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>BillingAddress</t>
+  </si>
+  <si>
+    <t>CreditCardNumber</t>
+  </si>
+  <si>
+    <t>CreditCardType</t>
+  </si>
+  <si>
+    <t>ExpiryMonth</t>
+  </si>
+  <si>
+    <t>ExpiryYear</t>
+  </si>
+  <si>
+    <t>CVV</t>
+  </si>
+  <si>
+    <t>Gudani</t>
+  </si>
+  <si>
+    <t>Manganye</t>
+  </si>
+  <si>
+    <t>13th Avenue, Sandton, 2196</t>
+  </si>
+  <si>
+    <t>5105105105105100</t>
+  </si>
+  <si>
+    <t>Master Card</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>2028</t>
+  </si>
+  <si>
+    <t>343</t>
   </si>
 </sst>
 </file>
@@ -86,9 +184,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,7 +470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -403,4 +502,158 @@
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;7&amp;K000000 C2 General</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34FC664E-1D0B-4675-8EC5-C70BFB9674D6}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{968887D1-7089-42A9-95FD-B3D9C911B76E}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>